<commit_message>
Backup folder - 2024-07-07 01:25:42
</commit_message>
<xml_diff>
--- a/Практика/Mentor Tasks/1.1/1.1.xlsx
+++ b/Практика/Mentor Tasks/1.1/1.1.xlsx
@@ -8,20 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yarik/Desktop/✈️ ХАІ 💻/Практика/Mentor Tasks/1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB1B675-5234-6246-872B-A920D88FAD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C71B62-527D-CE4F-8523-444EBA5C1E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{096DB306-C17B-0845-A1AC-1914401AB9D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$A$2:$A$33</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$B$2:$B$33</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$A$2:$A$33</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$B$2:$B$33</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1055,15 +1049,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1391,7 +1385,7 @@
   <dimension ref="A1:B106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,7 +1419,7 @@
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A67" si="0">A3+0.1</f>
+        <f t="shared" ref="A4:A33" si="0">A3+0.1</f>
         <v>0.2</v>
       </c>
       <c r="B4" s="2">

</xml_diff>